<commit_message>
valid and invalid creds check
</commit_message>
<xml_diff>
--- a/inputData/data.xlsx
+++ b/inputData/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAN\EWorkspace\TestPageFac\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A538E9-DC13-44B2-BBE0-1B7CFB8E8B5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB88202-0FE4-4ABD-85CE-B1B9939E5ACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="abc" sheetId="1" r:id="rId1"/>
+    <sheet name="validLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>mngr371386</t>
   </si>
   <si>
     <t>YhyrYvu</t>
+  </si>
+  <si>
+    <t>mngr377622</t>
+  </si>
+  <si>
+    <t>Avanapu</t>
   </si>
 </sst>
 </file>
@@ -357,13 +364,36 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B651AEF-032D-4F03-B013-E85CF16E3A1C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -374,7 +404,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
handeled new customer login
</commit_message>
<xml_diff>
--- a/inputData/data.xlsx
+++ b/inputData/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAN\EWorkspace\TestPageFac\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8838CC8B-B2EE-4F5B-9546-24F404A02CF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A40E0E4-E759-4293-9A13-4E1E9F19C89E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="15600" windowHeight="7236" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLogin" sheetId="1" r:id="rId1"/>
@@ -53,22 +53,22 @@
     <t>281992</t>
   </si>
   <si>
-    <t>manoj1@gmail.com</t>
-  </si>
-  <si>
-    <t>manoj2@gmail.com</t>
-  </si>
-  <si>
-    <t>manojl</t>
-  </si>
-  <si>
-    <t>manojm</t>
-  </si>
-  <si>
     <t>mngr391197</t>
   </si>
   <si>
     <t>AsuqeqE</t>
+  </si>
+  <si>
+    <t>manoj24@gmail.com</t>
+  </si>
+  <si>
+    <t>manoj25@gmail.com</t>
+  </si>
+  <si>
+    <t>manojkumari</t>
+  </si>
+  <si>
+    <t>manojkumarj</t>
   </si>
 </sst>
 </file>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,10 +406,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -444,15 +444,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0C0646-84DE-453A-8446-F045390EF0DD}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -473,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -481,7 +482,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -502,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
@@ -511,7 +512,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H1" r:id="rId1" display="manoj@gmail.com" xr:uid="{DE13859A-734A-4ABC-A74A-B2BD622D7C48}"/>
-    <hyperlink ref="H2" r:id="rId2" display="manoj@gmail.com" xr:uid="{087BB18F-AD57-4DD4-8B2A-F536F80D49DE}"/>
+    <hyperlink ref="H2" r:id="rId2" display="manoj@gmail.com" xr:uid="{5B69A65E-BE9D-4487-A9A7-5CDC3F57CE35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>